<commit_message>
Final Version of Ex1 and 2
</commit_message>
<xml_diff>
--- a/docs/Function Tables_ Exersice 1 and 2.xlsx
+++ b/docs/Function Tables_ Exersice 1 and 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\veron\Desktop\TEC\2022\ISemestre\TallerDigitales\Lab1\codigo\Taller-Digitales-LAB1\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A6556D-6874-46A7-80AE-1BA71449A06F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0004782E-7099-4692-9D37-EB95E4B0B61A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" activeTab="1" xr2:uid="{A9D623CC-A7E8-4794-BE06-D948F2752EAE}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
   <si>
     <t>One table works for all the groups</t>
   </si>
@@ -104,40 +104,34 @@
     <t>o</t>
   </si>
   <si>
-    <t>VARIABLE  MUX</t>
+    <t>ADDER</t>
   </si>
   <si>
-    <t>4 IN</t>
+    <t>A</t>
   </si>
   <si>
-    <t>OF VARIABLE WIDTH</t>
+    <t>B</t>
   </si>
   <si>
-    <t>1 OUT</t>
+    <t>Cin</t>
   </si>
   <si>
-    <t>A [N:0]</t>
+    <t>SUM</t>
   </si>
   <si>
-    <t>B[N:0]</t>
+    <t>Cout</t>
   </si>
   <si>
-    <t>C [N:0]</t>
+    <t>SUM :</t>
   </si>
   <si>
-    <t>D [N:0]</t>
+    <t>CinXOR(A XOR B)</t>
   </si>
   <si>
-    <t>ENABLE</t>
+    <t>Cout:</t>
   </si>
   <si>
-    <t>S0</t>
-  </si>
-  <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>Y [N:0]</t>
+    <t>CinB+A(Cin EXOR B)</t>
   </si>
 </sst>
 </file>
@@ -181,7 +175,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,8 +230,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -245,11 +257,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -266,6 +293,16 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -298,8 +335,8 @@
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="128240" cy="175113"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="CuadroTexto 2">
@@ -341,6 +378,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -373,7 +411,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="CuadroTexto 2">
@@ -443,8 +481,8 @@
       <xdr:rowOff>39688</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="CuadroTexto 3">
@@ -486,6 +524,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -524,7 +563,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="CuadroTexto 3">
@@ -600,8 +639,8 @@
       <xdr:rowOff>27781</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="CuadroTexto 4">
@@ -643,6 +682,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -681,7 +721,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="CuadroTexto 4">
@@ -757,8 +797,8 @@
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="CuadroTexto 5">
@@ -800,6 +840,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -838,7 +879,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="CuadroTexto 5">
@@ -972,8 +1013,8 @@
       <xdr:rowOff>41275</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="128240" cy="175113"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="CuadroTexto 8">
@@ -1015,6 +1056,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1047,7 +1089,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="CuadroTexto 8">
@@ -1117,8 +1159,8 @@
       <xdr:rowOff>49213</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="CuadroTexto 9">
@@ -1160,6 +1202,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1198,7 +1241,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="CuadroTexto 9">
@@ -1274,8 +1317,8 @@
       <xdr:rowOff>37306</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="CuadroTexto 10">
@@ -1317,6 +1360,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1355,7 +1399,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="CuadroTexto 10">
@@ -1489,8 +1533,8 @@
       <xdr:rowOff>30956</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="14" name="CuadroTexto 13">
@@ -1532,6 +1576,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1570,7 +1615,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="14" name="CuadroTexto 13">
@@ -1646,8 +1691,8 @@
       <xdr:rowOff>34925</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="128240" cy="175113"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="15" name="CuadroTexto 14">
@@ -1689,6 +1734,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1721,7 +1767,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="15" name="CuadroTexto 14">
@@ -1791,8 +1837,8 @@
       <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="16" name="CuadroTexto 15">
@@ -1834,6 +1880,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1872,7 +1919,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="16" name="CuadroTexto 15">
@@ -2006,8 +2053,8 @@
       <xdr:rowOff>28576</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="128240" cy="175113"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="20" name="CuadroTexto 19">
@@ -2049,6 +2096,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -2081,7 +2129,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="20" name="CuadroTexto 19">
@@ -2151,8 +2199,8 @@
       <xdr:rowOff>26988</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="128240" cy="175113"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="21" name="CuadroTexto 20">
@@ -2194,6 +2242,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -2226,7 +2275,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="21" name="CuadroTexto 20">
@@ -2296,8 +2345,8 @@
       <xdr:rowOff>20637</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="128240" cy="175113"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="22" name="CuadroTexto 21">
@@ -2339,6 +2388,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -2371,7 +2421,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="22" name="CuadroTexto 21">
@@ -2441,8 +2491,8 @@
       <xdr:rowOff>14288</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="128240" cy="175113"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="23" name="CuadroTexto 22">
@@ -2484,6 +2534,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -2516,7 +2567,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="23" name="CuadroTexto 22">
@@ -2586,8 +2637,8 @@
       <xdr:rowOff>27781</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="128240" cy="175113"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="24" name="CuadroTexto 23">
@@ -2629,6 +2680,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -2661,7 +2713,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="24" name="CuadroTexto 23">
@@ -2731,8 +2783,8 @@
       <xdr:rowOff>21431</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="128240" cy="175113"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="25" name="CuadroTexto 24">
@@ -2774,6 +2826,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -2806,7 +2859,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="25" name="CuadroTexto 24">
@@ -2876,8 +2929,8 @@
       <xdr:rowOff>15081</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="128240" cy="175113"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="26" name="CuadroTexto 25">
@@ -2919,6 +2972,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -2951,7 +3005,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="26" name="CuadroTexto 25">
@@ -3021,8 +3075,8 @@
       <xdr:rowOff>23813</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="128240" cy="175113"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="27" name="CuadroTexto 26">
@@ -3064,6 +3118,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -3096,7 +3151,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="27" name="CuadroTexto 26">
@@ -3166,8 +3221,8 @@
       <xdr:rowOff>17463</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="128240" cy="175113"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="28" name="CuadroTexto 27">
@@ -3209,6 +3264,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -3241,7 +3297,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="28" name="CuadroTexto 27">
@@ -3311,8 +3367,8 @@
       <xdr:rowOff>11114</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="128240" cy="175113"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="29" name="CuadroTexto 28">
@@ -3354,6 +3410,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -3386,7 +3443,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="29" name="CuadroTexto 28">
@@ -3456,8 +3513,8 @@
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="128240" cy="175113"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="30" name="CuadroTexto 29">
@@ -3499,6 +3556,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -3531,7 +3589,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="30" name="CuadroTexto 29">
@@ -3601,8 +3659,8 @@
       <xdr:rowOff>17462</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="128240" cy="175113"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="31" name="CuadroTexto 30">
@@ -3644,6 +3702,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -3676,7 +3735,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="31" name="CuadroTexto 30">
@@ -3746,8 +3805,8 @@
       <xdr:rowOff>47626</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="33" name="CuadroTexto 32">
@@ -3789,6 +3848,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -3827,7 +3887,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="33" name="CuadroTexto 32">
@@ -3903,8 +3963,8 @@
       <xdr:rowOff>57152</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="34" name="CuadroTexto 33">
@@ -3946,6 +4006,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -3984,7 +4045,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="34" name="CuadroTexto 33">
@@ -4060,8 +4121,8 @@
       <xdr:rowOff>26987</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="35" name="CuadroTexto 34">
@@ -4103,6 +4164,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -4141,7 +4203,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="35" name="CuadroTexto 34">
@@ -4217,8 +4279,8 @@
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="36" name="CuadroTexto 35">
@@ -4260,6 +4322,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -4298,7 +4361,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="36" name="CuadroTexto 35">
@@ -4374,8 +4437,8 @@
       <xdr:rowOff>27780</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="37" name="CuadroTexto 36">
@@ -4417,6 +4480,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -4455,7 +4519,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="37" name="CuadroTexto 36">
@@ -4531,8 +4595,8 @@
       <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="38" name="CuadroTexto 37">
@@ -4574,6 +4638,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -4612,7 +4677,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="38" name="CuadroTexto 37">
@@ -4688,8 +4753,8 @@
       <xdr:rowOff>42863</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="39" name="CuadroTexto 38">
@@ -4731,6 +4796,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -4769,7 +4835,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="39" name="CuadroTexto 38">
@@ -4845,8 +4911,8 @@
       <xdr:rowOff>36512</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="40" name="CuadroTexto 39">
@@ -4888,6 +4954,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -4926,7 +4993,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="40" name="CuadroTexto 39">
@@ -5002,8 +5069,8 @@
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="41" name="CuadroTexto 40">
@@ -5045,6 +5112,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -5083,7 +5151,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="41" name="CuadroTexto 40">
@@ -6377,8 +6445,8 @@
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="67" name="CuadroTexto 66">
@@ -6420,6 +6488,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -6458,7 +6527,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="67" name="CuadroTexto 66">
@@ -6534,8 +6603,8 @@
       <xdr:rowOff>30956</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="68" name="CuadroTexto 67">
@@ -6577,6 +6646,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -6615,7 +6685,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="68" name="CuadroTexto 67">
@@ -6691,8 +6761,8 @@
       <xdr:rowOff>37305</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="69" name="CuadroTexto 68">
@@ -6734,6 +6804,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -6772,7 +6843,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="69" name="CuadroTexto 68">
@@ -6848,8 +6919,8 @@
       <xdr:rowOff>35719</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="70" name="CuadroTexto 69">
@@ -6891,6 +6962,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -6929,7 +7001,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="70" name="CuadroTexto 69">
@@ -7353,8 +7425,8 @@
       <xdr:rowOff>50799</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="77" name="CuadroTexto 76">
@@ -7396,6 +7468,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -7434,7 +7507,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="77" name="CuadroTexto 76">
@@ -7510,8 +7583,8 @@
       <xdr:rowOff>49213</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="78" name="CuadroTexto 77">
@@ -7553,6 +7626,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -7591,7 +7665,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="78" name="CuadroTexto 77">
@@ -7667,8 +7741,8 @@
       <xdr:rowOff>19844</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="79" name="CuadroTexto 78">
@@ -7710,6 +7784,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -7748,7 +7823,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="79" name="CuadroTexto 78">
@@ -7824,8 +7899,8 @@
       <xdr:rowOff>18258</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="80" name="CuadroTexto 79">
@@ -7867,6 +7942,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -7905,7 +7981,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="80" name="CuadroTexto 79">
@@ -7981,8 +8057,8 @@
       <xdr:rowOff>30956</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="81" name="CuadroTexto 80">
@@ -8024,6 +8100,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -8062,7 +8139,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="81" name="CuadroTexto 80">
@@ -8196,8 +8273,8 @@
       <xdr:rowOff>31749</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="83" name="CuadroTexto 82">
@@ -8239,6 +8316,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -8277,7 +8355,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="83" name="CuadroTexto 82">
@@ -8411,8 +8489,8 @@
       <xdr:rowOff>43657</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="85" name="CuadroTexto 84">
@@ -8454,6 +8532,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -8492,7 +8571,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="85" name="CuadroTexto 84">
@@ -8626,8 +8705,8 @@
       <xdr:rowOff>15874</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="87" name="CuadroTexto 86">
@@ -8669,6 +8748,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -8707,7 +8787,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="87" name="CuadroTexto 86">
@@ -8841,8 +8921,8 @@
       <xdr:rowOff>15875</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="89" name="CuadroTexto 88">
@@ -8884,6 +8964,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -8922,7 +9003,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="89" name="CuadroTexto 88">
@@ -9056,8 +9137,8 @@
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="91" name="CuadroTexto 90">
@@ -9099,6 +9180,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -9137,7 +9219,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="91" name="CuadroTexto 90">
@@ -10141,8 +10223,8 @@
       <xdr:rowOff>39688</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="187" name="CuadroTexto 186">
@@ -10184,6 +10266,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -10222,7 +10305,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="187" name="CuadroTexto 186">
@@ -10298,8 +10381,8 @@
       <xdr:rowOff>27781</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="188" name="CuadroTexto 187">
@@ -10341,6 +10424,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -10379,7 +10463,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="188" name="CuadroTexto 187">
@@ -10455,8 +10539,8 @@
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="189" name="CuadroTexto 188">
@@ -10498,6 +10582,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -10536,7 +10621,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="189" name="CuadroTexto 188">
@@ -10670,8 +10755,8 @@
       <xdr:rowOff>49213</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="191" name="CuadroTexto 190">
@@ -10713,6 +10798,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -10751,7 +10837,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="191" name="CuadroTexto 190">
@@ -10827,8 +10913,8 @@
       <xdr:rowOff>37306</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="192" name="CuadroTexto 191">
@@ -10870,6 +10956,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -10908,7 +10995,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="192" name="CuadroTexto 191">
@@ -11042,8 +11129,8 @@
       <xdr:rowOff>30956</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="194" name="CuadroTexto 193">
@@ -11085,6 +11172,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -11123,7 +11211,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="194" name="CuadroTexto 193">
@@ -11199,8 +11287,8 @@
       <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="195" name="CuadroTexto 194">
@@ -11242,6 +11330,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -11280,7 +11369,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="195" name="CuadroTexto 194">
@@ -11414,8 +11503,8 @@
       <xdr:rowOff>47626</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="197" name="CuadroTexto 196">
@@ -11457,6 +11546,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -11495,7 +11585,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="197" name="CuadroTexto 196">
@@ -11571,8 +11661,8 @@
       <xdr:rowOff>57152</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="198" name="CuadroTexto 197">
@@ -11614,6 +11704,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -11652,7 +11743,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="198" name="CuadroTexto 197">
@@ -11728,8 +11819,8 @@
       <xdr:rowOff>26987</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="199" name="CuadroTexto 198">
@@ -11771,6 +11862,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -11809,7 +11901,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="199" name="CuadroTexto 198">
@@ -11885,8 +11977,8 @@
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="200" name="CuadroTexto 199">
@@ -11928,6 +12020,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -11966,7 +12059,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="200" name="CuadroTexto 199">
@@ -12042,8 +12135,8 @@
       <xdr:rowOff>27780</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="201" name="CuadroTexto 200">
@@ -12085,6 +12178,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -12123,7 +12217,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="201" name="CuadroTexto 200">
@@ -12199,8 +12293,8 @@
       <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="202" name="CuadroTexto 201">
@@ -12242,6 +12336,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -12280,7 +12375,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="202" name="CuadroTexto 201">
@@ -12356,8 +12451,8 @@
       <xdr:rowOff>42863</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="203" name="CuadroTexto 202">
@@ -12399,6 +12494,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -12437,7 +12533,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="203" name="CuadroTexto 202">
@@ -12513,8 +12609,8 @@
       <xdr:rowOff>36512</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="204" name="CuadroTexto 203">
@@ -12556,6 +12652,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -12594,7 +12691,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="204" name="CuadroTexto 203">
@@ -12670,8 +12767,8 @@
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="205" name="CuadroTexto 204">
@@ -12713,6 +12810,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -12751,7 +12849,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="205" name="CuadroTexto 204">
@@ -13813,8 +13911,8 @@
       <xdr:rowOff>37305</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="223" name="CuadroTexto 222">
@@ -13856,6 +13954,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -13894,7 +13993,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="223" name="CuadroTexto 222">
@@ -13970,8 +14069,8 @@
       <xdr:rowOff>35719</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="224" name="CuadroTexto 223">
@@ -14013,6 +14112,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -14051,7 +14151,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="224" name="CuadroTexto 223">
@@ -14475,8 +14575,8 @@
       <xdr:rowOff>50799</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="231" name="CuadroTexto 230">
@@ -14518,6 +14618,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -14556,7 +14657,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="231" name="CuadroTexto 230">
@@ -14632,8 +14733,8 @@
       <xdr:rowOff>49213</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="232" name="CuadroTexto 231">
@@ -14675,6 +14776,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -14713,7 +14815,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="232" name="CuadroTexto 231">
@@ -14789,8 +14891,8 @@
       <xdr:rowOff>19844</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="233" name="CuadroTexto 232">
@@ -14832,6 +14934,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -14870,7 +14973,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="233" name="CuadroTexto 232">
@@ -14946,8 +15049,8 @@
       <xdr:rowOff>18258</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="234" name="CuadroTexto 233">
@@ -14989,6 +15092,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -15027,7 +15131,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="234" name="CuadroTexto 233">
@@ -15103,8 +15207,8 @@
       <xdr:rowOff>30956</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="235" name="CuadroTexto 234">
@@ -15146,6 +15250,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -15184,7 +15289,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="235" name="CuadroTexto 234">
@@ -15318,8 +15423,8 @@
       <xdr:rowOff>31749</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="237" name="CuadroTexto 236">
@@ -15361,6 +15466,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -15399,7 +15505,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="237" name="CuadroTexto 236">
@@ -15533,8 +15639,8 @@
       <xdr:rowOff>43657</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="239" name="CuadroTexto 238">
@@ -15576,6 +15682,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -15614,7 +15721,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="239" name="CuadroTexto 238">
@@ -15748,8 +15855,8 @@
       <xdr:rowOff>15874</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="241" name="CuadroTexto 240">
@@ -15791,6 +15898,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -15829,7 +15937,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="241" name="CuadroTexto 240">
@@ -15963,8 +16071,8 @@
       <xdr:rowOff>15875</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="243" name="CuadroTexto 242">
@@ -16006,6 +16114,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -16044,7 +16153,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="243" name="CuadroTexto 242">
@@ -16178,8 +16287,8 @@
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184602" cy="176202"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="245" name="CuadroTexto 244">
@@ -16221,6 +16330,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -16259,7 +16369,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="245" name="CuadroTexto 244">
@@ -16385,6 +16495,475 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>120650</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>727075</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>168275</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectángulo 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D85EC0B8-84EA-44FB-920A-312027F9A005}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7620000" y="3784600"/>
+          <a:ext cx="606425" cy="130175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectángulo 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02768FC3-FEB1-4612-849A-75A069445F7E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8426450" y="3587750"/>
+          <a:ext cx="606425" cy="130175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>155575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectángulo 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CB9814E-804D-41C3-A09D-0B03F226023C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9169400" y="3771900"/>
+          <a:ext cx="606425" cy="130175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>739775</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectángulo 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFF085F7-4F61-40F5-A198-F4596036B5D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9918700" y="3590925"/>
+          <a:ext cx="606425" cy="130175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>650875</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>34925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectángulo 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CC32354-2432-4B2B-A035-E504EE6E5C47}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9674225" y="5280025"/>
+          <a:ext cx="936625" cy="149225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="accent2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>3175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>174625</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>174625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectángulo 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6019CA2-46A0-4AEB-9B26-D134E4147C35}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9353550" y="5060950"/>
+          <a:ext cx="606425" cy="358775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>501650</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectángulo 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{020DBECE-0B3A-4896-8F99-C0D277410789}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8763000" y="5270500"/>
+          <a:ext cx="1012825" cy="139700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -16685,29 +17264,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64005C75-FD86-496A-99C3-A03F89D6D33E}">
-  <dimension ref="A1:Z36"/>
+  <dimension ref="A1:AI36"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="AH7" sqref="AH7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="32.90625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="6.76953125" customWidth="1"/>
-    <col min="11" max="11" width="7.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="6.76953125" customWidth="1"/>
-    <col min="14" max="17" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="10.7265625" customWidth="1"/>
-    <col min="20" max="20" width="6.76953125" customWidth="1"/>
+    <col min="7" max="10" width="6.76953125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="7.08984375" hidden="1" customWidth="1"/>
+    <col min="12" max="13" width="6.76953125" hidden="1" customWidth="1"/>
+    <col min="14" max="19" width="10.7265625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="6.76953125" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="5.5" customWidth="1"/>
-    <col min="22" max="25" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.86328125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="14.1328125" customWidth="1"/>
     <col min="27" max="27" width="5.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16715,7 +17294,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -16741,7 +17320,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -16756,7 +17335,7 @@
       </c>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.75">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -16821,7 +17400,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.75">
       <c r="B5">
         <v>0</v>
       </c>
@@ -16886,7 +17465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.75">
       <c r="B6">
         <v>0</v>
       </c>
@@ -16954,7 +17533,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.75">
       <c r="B7">
         <v>0</v>
       </c>
@@ -17012,8 +17591,11 @@
       <c r="Z7" t="s">
         <v>12</v>
       </c>
+      <c r="AI7">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.75">
       <c r="B8">
         <v>0</v>
       </c>
@@ -17072,7 +17654,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.75">
       <c r="B9">
         <v>0</v>
       </c>
@@ -17131,7 +17713,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.75">
       <c r="B10">
         <v>0</v>
       </c>
@@ -17190,7 +17772,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.75">
       <c r="B11">
         <v>0</v>
       </c>
@@ -17249,7 +17831,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.75">
       <c r="B12">
         <v>0</v>
       </c>
@@ -17308,7 +17890,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.75">
       <c r="B13">
         <v>0</v>
       </c>
@@ -17367,7 +17949,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.75">
       <c r="B14">
         <v>0</v>
       </c>
@@ -17426,7 +18008,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.75">
       <c r="B15">
         <v>0</v>
       </c>
@@ -17485,7 +18067,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.75">
       <c r="B16">
         <v>0</v>
       </c>
@@ -18770,122 +19352,287 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B4BB45-3F08-445C-A5A0-831380A9DC00}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A3:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.6796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A1" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C4" t="s">
         <v>23</v>
       </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" s="17"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="J7" s="14">
+        <v>0</v>
+      </c>
+      <c r="K7" s="14">
+        <v>1</v>
+      </c>
+      <c r="L7" s="14">
+        <v>0</v>
+      </c>
+      <c r="M7" s="14">
+        <v>1</v>
+      </c>
+      <c r="O7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="I8" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B3" t="s">
+      <c r="J8" s="14">
+        <v>1</v>
+      </c>
+      <c r="K8" s="14">
+        <v>0</v>
+      </c>
+      <c r="L8" s="14">
+        <v>1</v>
+      </c>
+      <c r="M8" s="14">
+        <v>0</v>
+      </c>
+      <c r="O8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="I9" s="15"/>
+      <c r="K9" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="16"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="H13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="L14" s="17" t="s">
         <v>23</v>
       </c>
+      <c r="M14" s="17"/>
+      <c r="O14" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" t="s">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="J15" s="14">
+        <v>0</v>
+      </c>
+      <c r="K15" s="14">
+        <v>0</v>
+      </c>
+      <c r="L15" s="14">
+        <v>1</v>
+      </c>
+      <c r="M15" s="14">
+        <v>0</v>
+      </c>
+      <c r="O15" t="s">
         <v>30</v>
       </c>
-      <c r="F5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" t="s">
-        <v>32</v>
-      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6" t="s">
-        <v>25</v>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="I16" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J16" s="14">
+        <v>0</v>
+      </c>
+      <c r="K16" s="14">
+        <v>1</v>
+      </c>
+      <c r="L16" s="14">
+        <v>1</v>
+      </c>
+      <c r="M16" s="14">
+        <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>28</v>
-      </c>
+    <row r="17" spans="9:12" x14ac:dyDescent="0.75">
+      <c r="I17" s="15"/>
+      <c r="K17" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" s="16"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="K17:L17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>